<commit_message>
change FeatureCollection options and cleanup
</commit_message>
<xml_diff>
--- a/my_xlsx/SheetJSExportAOO.xlsx
+++ b/my_xlsx/SheetJSExportAOO.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,6 +454,9 @@
       <c r="Q1" t="str">
         <v>ORG_N</v>
       </c>
+      <c r="R1" t="str">
+        <v>Id</v>
+      </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
@@ -508,10 +511,13 @@
       <c r="Q2" t="str">
         <v>101-0925198</v>
       </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:R2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>